<commit_message>
Update species list to 1.3.1 for NE
</commit_message>
<xml_diff>
--- a/Species Lists & Guides by Region/New England Species List v1.3.1.xlsx
+++ b/Species Lists & Guides by Region/New England Species List v1.3.1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26024"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26929"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22040" yWindow="2900" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Complete_GOM_Taxa" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="755">
   <si>
     <t>sea cauliflower</t>
   </si>
@@ -2353,6 +2353,18 @@
   </si>
   <si>
     <t>Added common division name column</t>
+  </si>
+  <si>
+    <t>HESN</t>
+  </si>
+  <si>
+    <t>Hemigrapsus sanguinolenta</t>
+  </si>
+  <si>
+    <t>Asian invasive crab</t>
+  </si>
+  <si>
+    <t>banded legs, small</t>
   </si>
 </sst>
 </file>
@@ -3386,8 +3398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6755,10 +6767,19 @@
       <c r="AR113" s="36"/>
     </row>
     <row r="114" spans="1:44">
-      <c r="D114" s="19"/>
-      <c r="E114" s="31"/>
+      <c r="D114" s="46" t="s">
+        <v>751</v>
+      </c>
+      <c r="E114" s="31" t="s">
+        <v>752</v>
+      </c>
       <c r="F114" s="3"/>
-      <c r="H114" s="5"/>
+      <c r="G114" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="H114" s="5" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="115" spans="1:44">
       <c r="B115" s="3"/>

</xml_diff>